<commit_message>
modified:   052350-9/052350-9R Axis Apollo Controller.pcb 	modified:   052350-9/052350-9R Axis Apollo Main Schematic.sch
</commit_message>
<xml_diff>
--- a/052350-9/Manufacture/BillOfMaterials.rep.xlsx
+++ b/052350-9/Manufacture/BillOfMaterials.rep.xlsx
@@ -127,25 +127,7 @@
     <t xml:space="preserve">Z357PA40-SMT-P-NC-N</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://www.digikey.ca/products/en?keywords=Z357PA40-SMT-P-NC-N</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
+    <t xml:space="preserve">https://www.digikey.ca/products/en?keywords=Z357PA40-SMT-P-NC-N </t>
   </si>
   <si>
     <t xml:space="preserve">U12</t>
@@ -178,25 +160,7 @@
     <t xml:space="preserve">ERJ-6DQF1R3V</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://www.digikey.ca/product-detail/en/panasonic-electronic-components/ERJ-6DQF1R3V/P19271CT-ND/6004626</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
+    <t xml:space="preserve">https://www.digikey.ca/product-detail/en/panasonic-electronic-components/ERJ-6DQF1R3V/P19271CT-ND/6004626 </t>
   </si>
   <si>
     <t xml:space="preserve">R21 R43 R44 R46 R47</t>
@@ -247,25 +211,7 @@
     <t xml:space="preserve">RMCF0603FT7M50</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://www.digikey.ca/product-detail/en/stackpole-electronics-inc/RMCF0603FT7M50/RMCF0603FT7M50CT-ND/7790073</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
+    <t xml:space="preserve">https://www.digikey.ca/product-detail/en/stackpole-electronics-inc/RMCF0603FT7M50/RMCF0603FT7M50CT-ND/7790073 </t>
   </si>
   <si>
     <t xml:space="preserve">R69</t>
@@ -292,25 +238,7 @@
     <t xml:space="preserve">CRCW0603174KFKEA</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://www.digikey.ca/product-detail/en/vishay-dale/CRCW0603174KFKEA/541-174KHCT-ND/1180063</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
+    <t xml:space="preserve">https://www.digikey.ca/product-detail/en/vishay-dale/CRCW0603174KFKEA/541-174KHCT-ND/1180063 </t>
   </si>
   <si>
     <t xml:space="preserve">R28</t>
@@ -367,25 +295,7 @@
     <t xml:space="preserve">CRCW06031K65FKEA</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://www.digikey.ca/product-detail/en/vishay-dale/CRCW06031K65FKEA/541-1.65KHDKR-ND/1184965</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
+    <t xml:space="preserve">https://www.digikey.ca/product-detail/en/vishay-dale/CRCW06031K65FKEA/541-1.65KHDKR-ND/1184965 </t>
   </si>
   <si>
     <t xml:space="preserve">R10</t>
@@ -400,25 +310,7 @@
     <t xml:space="preserve">RMCF0603FT2M37</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://www.digikey.ca/product-detail/en/stackpole-electronics-inc/RMCF0603FT2M37/RMCF0603FT2M37CT-ND/7790160</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
+    <t xml:space="preserve">https://www.digikey.ca/product-detail/en/stackpole-electronics-inc/RMCF0603FT2M37/RMCF0603FT2M37CT-ND/7790160 </t>
   </si>
   <si>
     <t xml:space="preserve">R7 R30 R32 R33 R36 R72</t>
@@ -725,8 +617,8 @@
   </sheetPr>
   <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B10" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D42" activeCellId="0" sqref="D42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B64" activeCellId="0" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1593,12 +1485,12 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D5" r:id="rId1" display="https://cdn-shop.adafruit.com/product-files/2686/SK6812MINI_REV.01-1-2.pdf"/>
-    <hyperlink ref="D16" r:id="rId2" display="https://www.digikey.ca/products/en?keywords=Z357PA40-SMT-P-NC-N"/>
-    <hyperlink ref="D21" r:id="rId3" display="https://www.digikey.ca/product-detail/en/panasonic-electronic-components/ERJ-6DQF1R3V/P19271CT-ND/6004626"/>
-    <hyperlink ref="D29" r:id="rId4" display="https://www.digikey.ca/product-detail/en/stackpole-electronics-inc/RMCF0603FT7M50/RMCF0603FT7M50CT-ND/7790073"/>
-    <hyperlink ref="D33" r:id="rId5" display="https://www.digikey.ca/product-detail/en/vishay-dale/CRCW0603174KFKEA/541-174KHCT-ND/1180063"/>
-    <hyperlink ref="D42" r:id="rId6" display="https://www.digikey.ca/product-detail/en/vishay-dale/CRCW06031K65FKEA/541-1.65KHDKR-ND/1184965"/>
-    <hyperlink ref="D44" r:id="rId7" display="https://www.digikey.ca/product-detail/en/stackpole-electronics-inc/RMCF0603FT2M37/RMCF0603FT2M37CT-ND/7790160"/>
+    <hyperlink ref="D16" r:id="rId2" display="https://www.digikey.ca/products/en?keywords=Z357PA40-SMT-P-NC-N "/>
+    <hyperlink ref="D21" r:id="rId3" display="https://www.digikey.ca/product-detail/en/panasonic-electronic-components/ERJ-6DQF1R3V/P19271CT-ND/6004626 "/>
+    <hyperlink ref="D29" r:id="rId4" display="https://www.digikey.ca/product-detail/en/stackpole-electronics-inc/RMCF0603FT7M50/RMCF0603FT7M50CT-ND/7790073 "/>
+    <hyperlink ref="D33" r:id="rId5" display="https://www.digikey.ca/product-detail/en/vishay-dale/CRCW0603174KFKEA/541-174KHCT-ND/1180063 "/>
+    <hyperlink ref="D42" r:id="rId6" display="https://www.digikey.ca/product-detail/en/vishay-dale/CRCW06031K65FKEA/541-1.65KHDKR-ND/1184965 "/>
+    <hyperlink ref="D44" r:id="rId7" display="https://www.digikey.ca/product-detail/en/stackpole-electronics-inc/RMCF0603FT2M37/RMCF0603FT2M37CT-ND/7790160 "/>
     <hyperlink ref="D63" r:id="rId8" display="http://www.huakevision.com/h-pd-634.html"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>